<commit_message>
Adding more test cases and POST request with invalid date to return 422 status code
</commit_message>
<xml_diff>
--- a/Checklist, Test Cases and RTM.xlsx
+++ b/Checklist, Test Cases and RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gdemirev/Desktop/the-movies-library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA99BD46-AABE-D042-AAF2-E85730550643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEE5744-38AC-5340-8CE5-1497610659CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{CA6878E5-EE3D-C843-BAFC-7E3E82FB860F}"/>
+    <workbookView xWindow="-51200" yWindow="-6460" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{CA6878E5-EE3D-C843-BAFC-7E3E82FB860F}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="143">
   <si>
     <t>Checklist - The Movie Library</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Automated</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>TC002</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Verify GET /movies/:id/edit Endpoint</t>
   </si>
   <si>
-    <t>Ensure the GET /movies/:id/edit endpoint returns the movie data for editing</t>
-  </si>
-  <si>
     <t>1. Send a POST request to /movies with valid movie data                                                  2. Verify the response status code is 200                  3. Verify the response body contains the created movie data</t>
   </si>
   <si>
@@ -310,46 +304,180 @@
     <t>Requirements Traceability Matrix (RTM)</t>
   </si>
   <si>
-    <t>Verify GET /movies</t>
-  </si>
-  <si>
-    <t>Verify POST /movies</t>
-  </si>
-  <si>
-    <t>Verify GET /movies/:id/edit</t>
-  </si>
-  <si>
-    <t>Verify PATCH /movies/:id</t>
-  </si>
-  <si>
-    <t>Verify DELETE /movies/:id</t>
-  </si>
-  <si>
-    <t>Verify GET /movies/search</t>
-  </si>
-  <si>
-    <t>Verify GET /movies/sort</t>
-  </si>
-  <si>
-    <t>Verify GET /actors</t>
-  </si>
-  <si>
-    <t>Verify POST /actors</t>
-  </si>
-  <si>
-    <t>Verify GET /actors/:id/edit</t>
-  </si>
-  <si>
-    <t>Verify PATCH /actors/:id</t>
-  </si>
-  <si>
-    <t>Verify DELETE /actors/:id</t>
-  </si>
-  <si>
-    <t>Verify GET /actors/search</t>
-  </si>
-  <si>
-    <t>Verify GET /actors/sort</t>
+    <t>Verify PATCH /movies/:id Endpoint</t>
+  </si>
+  <si>
+    <t>Verify GET /movies/search Endpoint</t>
+  </si>
+  <si>
+    <t>Verify GET /movies/sort Endpoint</t>
+  </si>
+  <si>
+    <t>Verify GET /actors Endpoint</t>
+  </si>
+  <si>
+    <t>Verify POST /actors Endpoint</t>
+  </si>
+  <si>
+    <t>Verify GET /actors/:id/edit Endpoint</t>
+  </si>
+  <si>
+    <t>Verify PATCH /actors/:id Endpoint</t>
+  </si>
+  <si>
+    <t>Verify DELETE /actors/:id Endpoint</t>
+  </si>
+  <si>
+    <t>Verify GET /actors/search Endpoint</t>
+  </si>
+  <si>
+    <t>Verify GET /actors/sort Endpoint</t>
+  </si>
+  <si>
+    <t>Ensure the GET /movies/search endpoint filters movies based on specified criteria</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains a list of movies that match the search criteria.</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify GET /movies/sort Endpoint</t>
+  </si>
+  <si>
+    <t>Ensure the GET /movies/sort endpoint sorts movies based on specified criteria</t>
+  </si>
+  <si>
+    <t>1. Authorize 2.Movies exist in the database</t>
+  </si>
+  <si>
+    <t>1. Authorize        2. Movie exist in the database</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /movies/sort with a valid sort parameter (e.g., name).
+2. Verify the response status code is 200.
+3. Verify the response body contains a sorted list of movies based on the specified criteria</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains a sorted list of movies</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /movies/search with a valid search parameter (e.g., id)
+2. Verify the response status code is 200.
+3. Verify the response body contains a list of movies that match the search criteria</t>
+  </si>
+  <si>
+    <t>Ensure the GET /actors endpoint returns a list of actors</t>
+  </si>
+  <si>
+    <t>1. Authorize         2. Actors exist in the database</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /actors                                          2. Verify the response status code is 200                 3. Verify the response body contains a list of actors</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains a list of actors</t>
+  </si>
+  <si>
+    <t>Ensure the POST /actors endpoint creates a new actor</t>
+  </si>
+  <si>
+    <t>1. Send a POST request to /actors with valid movie data                                                  2. Verify the response status code is 200                  3. Verify the response body contains the created actor data</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains the created actor data</t>
+  </si>
+  <si>
+    <t>1. Authorize       2. An actor with the specified ID exists in the database</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /actors/:id/edit with a valid movie ID                                          2. Verify the response status code is 200                 3. Verify the response body contains the actor data</t>
+  </si>
+  <si>
+    <t>Ensure the GET /movies/:id/edit endpoint edit the movie data for editing</t>
+  </si>
+  <si>
+    <t>Ensure the GET /actors/:id/edit endpoint returns the actor data for editing</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains the actor data</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains the movie data</t>
+  </si>
+  <si>
+    <t>1. Authorize        2. An actor with the specified ID exists in the database</t>
+  </si>
+  <si>
+    <t>1. Send a DELETE request to /actor/:id with a valid actor ID                                       2. Verify the response status code is 200                 3. Verify the response body contains a success message</t>
+  </si>
+  <si>
+    <t>Ensure the DELETE /actors/:id endpoint deletes the specified actor</t>
+  </si>
+  <si>
+    <t>Ensure the GET /actors/search endpoint filters movies based on specified criteria</t>
+  </si>
+  <si>
+    <t>1. Authorize        2. Actor exist in the database</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /actors/search with a valid search parameter (e.g., birtdate)
+2. Verify the response status code is 200.
+3. Verify the response body contains a list of movies that match the search criteria</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains a list of actors that match the search criteria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify GET /actors/sort Endpoint</t>
+  </si>
+  <si>
+    <t>Ensure the GET /actors/sort endpoint sorts actors based on specified criteria</t>
+  </si>
+  <si>
+    <t>1. Authorize 2.Actors exist in the database</t>
+  </si>
+  <si>
+    <t>The response status code is 200, and the response body contains a sorted list of actors</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /actors/sort with a valid sort parameter (e.g., id).
+2. Verify the response status code is 200.
+3. Verify the response body contains a sorted list of actors based on the specified criteria</t>
+  </si>
+  <si>
+    <t>The response status code is 404, and the response body contains an error message indicating that the movie was not found</t>
+  </si>
+  <si>
+    <t>Ensure the GET /movies/search endpoint returns an error when an invalid movie name is provided</t>
+  </si>
+  <si>
+    <t>Verify POST /movies with Invalid Data</t>
+  </si>
+  <si>
+    <t>Ensure the POST /movies endpoint returns an error when invalid data is provided</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /movies/search?search="Test Movie" (assuming Test Movie is and invalid Name)                2. Verify the response status code is 404                                 3. Verify the response body contains an error message</t>
+  </si>
+  <si>
+    <t>1. Send a POST request to /movies with invalid movie data
+2. Verify the response status code in 422
+3. Verify the response body contains an error message</t>
+  </si>
+  <si>
+    <t>The response status code is 422, and the response body contains an error message indicating the validation errors</t>
+  </si>
+  <si>
+    <t>Ensure the GET /actors/search endpoint returns an error when an invalid actor name is provided</t>
+  </si>
+  <si>
+    <t>1. Send a GET request to /movies/search?search="Test Actor" (assuming Test Actor is and invalid Name)
+ 2. Verify the response status code is 404                                 3. Verify the response body contains an error message</t>
+  </si>
+  <si>
+    <t>TC015</t>
   </si>
 </sst>
 </file>
@@ -449,9 +577,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -484,6 +609,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,14 +621,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,26 +966,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803471BE-DB95-F54A-8FEA-703D3D7FBD0F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="22">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="19">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -871,7 +999,7 @@
       <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="19">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -885,7 +1013,7 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="19">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
@@ -899,7 +1027,7 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="19">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -913,7 +1041,7 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="19">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -927,7 +1055,7 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="19">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -941,7 +1069,7 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="19">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -955,7 +1083,7 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="19">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -970,6 +1098,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B8:H8"/>
@@ -978,7 +1107,6 @@
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -986,27 +1114,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6C98CD-71B6-2146-AB6A-DB44E2C7A397}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="26" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1015,174 +1143,428 @@
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" ht="26" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" s="11" customFormat="1" ht="26" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" s="11" customFormat="1" ht="26" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" s="11" customFormat="1" ht="26" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="26" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" ht="26" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="33" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="117" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="128" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="128" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="G7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="135" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="135" customHeight="1">
-      <c r="A8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="127" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="127" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="G9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="195" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="195" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="117" customHeight="1">
+      <c r="A12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="128" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="135" customHeight="1">
+      <c r="A14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="127" customHeight="1">
+      <c r="A15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="195" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="195" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="171" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="150" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="171" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1199,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361FBCF-5CA4-0D46-8ED5-48D78DE833CA}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1213,224 +1595,224 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="A1" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" ht="19">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="40">
+      <c r="A3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="40">
+      <c r="A4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60">
+      <c r="A5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20">
-      <c r="A3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="C5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="40">
+      <c r="A6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="40">
+      <c r="A7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60">
+      <c r="A8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="40">
+      <c r="A9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20">
-      <c r="A4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="15" t="s">
+    <row r="10" spans="1:4" ht="40">
+      <c r="A10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40">
-      <c r="A5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="15" t="s">
+    <row r="11" spans="1:4" ht="40">
+      <c r="A11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="40">
-      <c r="A6" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="15" t="s">
+    <row r="12" spans="1:4" ht="60">
+      <c r="A12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="40">
-      <c r="A7" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="15" t="s">
+    <row r="13" spans="1:4" ht="40">
+      <c r="A13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60">
-      <c r="A8" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="10" t="s">
+    <row r="14" spans="1:4" ht="40">
+      <c r="A14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="40">
-      <c r="A9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="15" t="s">
+    <row r="15" spans="1:4" ht="60">
+      <c r="A15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20">
-      <c r="A10" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="15" t="s">
+    <row r="16" spans="1:4" ht="40">
+      <c r="A16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20">
-      <c r="A11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="40">
-      <c r="A12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="40">
-      <c r="A13" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="40">
-      <c r="A14" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60">
-      <c r="A15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="40">
-      <c r="A16" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="17" spans="3:3" ht="20">
-      <c r="C17" s="4"/>
+      <c r="C17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>